<commit_message>
Updated group time sheets, fixed template and window issues in excel
</commit_message>
<xml_diff>
--- a/docs/project management/completed sheets/26.10.15/David_Fairbrother_timesheet.xlsx
+++ b/docs/project management/completed sheets/26.10.15/David_Fairbrother_timesheet.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -80,9 +80,6 @@
   </si>
   <si>
     <t>Create weekly report for meeting on Friday as per SE.QA.02</t>
-  </si>
-  <si>
-    <t>Todo</t>
   </si>
 </sst>
 </file>
@@ -480,7 +477,7 @@
       <pane xSplit="8" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,11 +513,11 @@
       </c>
       <c r="G1" s="4" t="str">
         <f>"Total hours accounted this week: " &amp;TEXT(I1, "hh:mm")</f>
-        <v>Total hours accounted this week: 02:00</v>
+        <v>Total hours accounted this week: 03:00</v>
       </c>
       <c r="I1" s="6">
         <f>SUM(F3:F100)</f>
-        <v>8.3333333333333329E-2</v>
+        <v>0.125</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -614,11 +611,11 @@
       <c r="D5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>21</v>
+      <c r="E5" s="10">
+        <v>42305</v>
+      </c>
+      <c r="F5" s="11">
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>

</xml_diff>